<commit_message>
Add plots for: SMD, eCDF and ORs
</commit_message>
<xml_diff>
--- a/3_intermediate/OR_import.xlsx
+++ b/3_intermediate/OR_import.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="11_88D1FD514068A76A5F098802EB9E65EADBDC33C4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED8ACDB4-862F-44AB-B542-04515194D176}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="5415" yWindow="1065" windowWidth="16140" windowHeight="14730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="28">
   <si>
     <t>OR</t>
   </si>
@@ -36,73 +37,79 @@
     <t>higher</t>
   </si>
   <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Urban/Rural: Urban Core</t>
-  </si>
-  <si>
-    <t>Urban/Rural: Urban Fringe</t>
-  </si>
-  <si>
-    <t>Urban/Rural: Urban out CMA/CAs</t>
-  </si>
-  <si>
-    <t>Urban/Rural: 2nd Urban Core</t>
-  </si>
-  <si>
-    <t>Urban/Rural: DA Only</t>
-  </si>
-  <si>
-    <t>Race: Non-White</t>
-  </si>
-  <si>
-    <t>Sex: Male</t>
-  </si>
-  <si>
-    <t>Education: High School</t>
-  </si>
-  <si>
-    <t>Education: Vocational Tr</t>
-  </si>
-  <si>
-    <t>Education: Non-Uni Cert</t>
-  </si>
-  <si>
-    <t>Education: Bachelor</t>
-  </si>
-  <si>
-    <t>Education: Graduate</t>
-  </si>
-  <si>
     <t>Depression Scale</t>
   </si>
   <si>
     <t>Vaccination &gt;15 Days</t>
   </si>
   <si>
-    <t>Prov Group: NF &amp; NS</t>
-  </si>
-  <si>
-    <t>Prov Group: QC</t>
-  </si>
-  <si>
-    <t>Prov Group: ON</t>
-  </si>
-  <si>
-    <t>Prov Group: MT &amp; AB</t>
-  </si>
-  <si>
     <t>Outbreak Peak</t>
   </si>
   <si>
     <t>Traveling Distance (km)</t>
+  </si>
+  <si>
+    <t>Unadjusted</t>
+  </si>
+  <si>
+    <t>Adjusted</t>
+  </si>
+  <si>
+    <t>Non-White (ref: White)</t>
+  </si>
+  <si>
+    <t>Prov Group: NF &amp; NS (ref: BC)</t>
+  </si>
+  <si>
+    <t>Sex: Male (ref: Female)</t>
+  </si>
+  <si>
+    <t>Age in 10-year scale</t>
+  </si>
+  <si>
+    <t>Prov Group: QC (ref: BC)</t>
+  </si>
+  <si>
+    <t>Prov Group: ON (ref: BC)</t>
+  </si>
+  <si>
+    <t>Prov Group: MT &amp; AB (ref: BC)</t>
+  </si>
+  <si>
+    <t>U/R: Urban Core (ref: Rural)</t>
+  </si>
+  <si>
+    <t>U/R: Urban Fringe (ref: Rural)</t>
+  </si>
+  <si>
+    <t>U/R: Urban out CMA/CAs (ref: Rural)</t>
+  </si>
+  <si>
+    <t>U/R: 2nd Urban Core (ref: Rural)</t>
+  </si>
+  <si>
+    <t>U/R: DA Only (ref: Rural)</t>
+  </si>
+  <si>
+    <t>Edu: High School (ref: &lt;High School)</t>
+  </si>
+  <si>
+    <t>Edu: Vocational Tr (ref: &lt;High School)</t>
+  </si>
+  <si>
+    <t>Edu: Non-Uni Cert (ref: &lt;High School)</t>
+  </si>
+  <si>
+    <t>Edu: Bachelor (ref: &lt;High School)</t>
+  </si>
+  <si>
+    <t>Edu: Graduate (ref: &lt;High School)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -149,6 +156,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -413,16 +424,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="40" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
@@ -447,24 +458,24 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B2">
-        <v>1.0036</v>
+        <v>1.04</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="D2">
-        <v>1.01</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>1.1200000000000001</v>
@@ -475,13 +486,13 @@
       <c r="D3">
         <v>1.23</v>
       </c>
-      <c r="E3">
-        <v>0</v>
+      <c r="E3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>0.87</v>
@@ -492,13 +503,13 @@
       <c r="D4">
         <v>1.05</v>
       </c>
-      <c r="E4">
-        <v>0</v>
+      <c r="E4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>0.88</v>
@@ -509,13 +520,13 @@
       <c r="D5">
         <v>1.26</v>
       </c>
-      <c r="E5">
-        <v>0</v>
+      <c r="E5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <v>1.49</v>
@@ -526,13 +537,13 @@
       <c r="D6">
         <v>2.86</v>
       </c>
-      <c r="E6">
-        <v>0</v>
+      <c r="E6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <v>0.38</v>
@@ -543,13 +554,13 @@
       <c r="D7">
         <v>0.57999999999999996</v>
       </c>
-      <c r="E7">
-        <v>0</v>
+      <c r="E7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>0.8</v>
@@ -560,8 +571,8 @@
       <c r="D8">
         <v>1.21</v>
       </c>
-      <c r="E8">
-        <v>0</v>
+      <c r="E8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -577,13 +588,13 @@
       <c r="D9">
         <v>0.8</v>
       </c>
-      <c r="E9">
-        <v>0</v>
+      <c r="E9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B10">
         <v>1.38</v>
@@ -594,13 +605,13 @@
       <c r="D10">
         <v>1.81</v>
       </c>
-      <c r="E10">
-        <v>0</v>
+      <c r="E10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B11">
         <v>1.1000000000000001</v>
@@ -611,13 +622,13 @@
       <c r="D11">
         <v>1.47</v>
       </c>
-      <c r="E11">
-        <v>0</v>
+      <c r="E11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B12">
         <v>0.91</v>
@@ -628,13 +639,13 @@
       <c r="D12">
         <v>1.19</v>
       </c>
-      <c r="E12">
-        <v>0</v>
+      <c r="E12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B13">
         <v>1.35</v>
@@ -645,13 +656,13 @@
       <c r="D13">
         <v>1.74</v>
       </c>
-      <c r="E13">
-        <v>0</v>
+      <c r="E13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B14">
         <v>1.27</v>
@@ -662,13 +673,13 @@
       <c r="D14">
         <v>1.64</v>
       </c>
-      <c r="E14">
-        <v>0</v>
+      <c r="E14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -679,13 +690,13 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15">
-        <v>0</v>
+      <c r="E15" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B16">
         <v>0.97340000000000004</v>
@@ -696,13 +707,13 @@
       <c r="D16">
         <v>0.98</v>
       </c>
-      <c r="E16">
-        <v>0</v>
+      <c r="E16" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B17">
         <v>0.62</v>
@@ -713,13 +724,13 @@
       <c r="D17">
         <v>0.68</v>
       </c>
-      <c r="E17">
-        <v>0</v>
+      <c r="E17" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B18">
         <v>1.63</v>
@@ -730,13 +741,13 @@
       <c r="D18">
         <v>1.9</v>
       </c>
-      <c r="E18">
-        <v>0</v>
+      <c r="E18" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B19">
         <v>0.72</v>
@@ -747,13 +758,13 @@
       <c r="D19">
         <v>0.84</v>
       </c>
-      <c r="E19">
-        <v>0</v>
+      <c r="E19" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B20">
         <v>2.14</v>
@@ -764,13 +775,13 @@
       <c r="D20">
         <v>2.4700000000000002</v>
       </c>
-      <c r="E20">
-        <v>0</v>
+      <c r="E20" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B21">
         <v>1.94</v>
@@ -781,13 +792,13 @@
       <c r="D21">
         <v>2.25</v>
       </c>
-      <c r="E21">
-        <v>0</v>
+      <c r="E21" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B22">
         <v>2.1800000000000002</v>
@@ -798,30 +809,30 @@
       <c r="D22">
         <v>2.74</v>
       </c>
-      <c r="E22">
-        <v>0</v>
+      <c r="E22" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B23">
-        <v>1.0037</v>
+        <v>1.04</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="D23">
-        <v>1.01</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B24">
         <v>1.1000000000000001</v>
@@ -832,13 +843,13 @@
       <c r="D24">
         <v>1.21</v>
       </c>
-      <c r="E24">
-        <v>1</v>
+      <c r="E24" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B25">
         <v>0.49</v>
@@ -849,13 +860,13 @@
       <c r="D25">
         <v>0.61</v>
       </c>
-      <c r="E25">
-        <v>1</v>
+      <c r="E25" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B26">
         <v>0.66</v>
@@ -866,30 +877,30 @@
       <c r="D26">
         <v>0.97</v>
       </c>
-      <c r="E26">
-        <v>1</v>
+      <c r="E26" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B27">
-        <v>1.61</v>
+        <v>1.59</v>
       </c>
       <c r="C27">
-        <v>0.83</v>
+        <v>0.82</v>
       </c>
       <c r="D27">
-        <v>3.21</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
+        <v>3.17</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B28">
         <v>0.51</v>
@@ -900,13 +911,13 @@
       <c r="D28">
         <v>0.79</v>
       </c>
-      <c r="E28">
-        <v>1</v>
+      <c r="E28" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B29">
         <v>0.47</v>
@@ -917,8 +928,8 @@
       <c r="D29">
         <v>0.73</v>
       </c>
-      <c r="E29">
-        <v>1</v>
+      <c r="E29" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -926,72 +937,72 @@
         <v>11</v>
       </c>
       <c r="B30">
-        <v>0.75</v>
+        <v>0.76</v>
       </c>
       <c r="C30">
         <v>0.56999999999999995</v>
       </c>
       <c r="D30">
-        <v>0.99</v>
-      </c>
-      <c r="E30">
         <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B31">
-        <v>1.38</v>
+        <v>1.37</v>
       </c>
       <c r="C31">
         <v>1.03</v>
       </c>
       <c r="D31">
-        <v>1.84</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
+        <v>1.83</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B32">
-        <v>1.1000000000000001</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="C32">
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
       <c r="D32">
-        <v>1.51</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
+        <v>1.52</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B33">
-        <v>0.92</v>
+        <v>0.91</v>
       </c>
       <c r="C33">
-        <v>0.7</v>
+        <v>0.69</v>
       </c>
       <c r="D33">
-        <v>1.23</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
+        <v>1.21</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B34">
         <v>1.26</v>
@@ -1002,30 +1013,30 @@
       <c r="D34">
         <v>1.66</v>
       </c>
-      <c r="E34">
-        <v>1</v>
+      <c r="E34" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B35">
-        <v>1.1399999999999999</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="C35">
-        <v>0.87</v>
+        <v>0.88</v>
       </c>
       <c r="D35">
-        <v>1.51</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
+        <v>1.52</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -1036,13 +1047,13 @@
       <c r="D36">
         <v>1</v>
       </c>
-      <c r="E36">
-        <v>1</v>
+      <c r="E36" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B37">
         <v>0.96</v>
@@ -1053,13 +1064,13 @@
       <c r="D37">
         <v>0.97</v>
       </c>
-      <c r="E37">
-        <v>1</v>
+      <c r="E37" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B38">
         <v>0.64</v>
@@ -1070,13 +1081,13 @@
       <c r="D38">
         <v>0.71</v>
       </c>
-      <c r="E38">
-        <v>1</v>
+      <c r="E38" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B39">
         <v>1.48</v>
@@ -1087,13 +1098,13 @@
       <c r="D39">
         <v>1.73</v>
       </c>
-      <c r="E39">
-        <v>1</v>
+      <c r="E39" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B40">
         <v>0.77</v>
@@ -1104,13 +1115,13 @@
       <c r="D40">
         <v>0.9</v>
       </c>
-      <c r="E40">
-        <v>1</v>
+      <c r="E40" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B41">
         <v>2.52</v>
@@ -1121,16 +1132,16 @@
       <c r="D41">
         <v>2.94</v>
       </c>
-      <c r="E41">
-        <v>1</v>
+      <c r="E41" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B42">
-        <v>2.0299999999999998</v>
+        <v>2.04</v>
       </c>
       <c r="C42">
         <v>1.74</v>
@@ -1138,25 +1149,25 @@
       <c r="D42">
         <v>2.38</v>
       </c>
-      <c r="E42">
-        <v>1</v>
+      <c r="E42" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B43">
         <v>1.73</v>
       </c>
       <c r="C43">
-        <v>1.37</v>
+        <v>1.36</v>
       </c>
       <c r="D43">
-        <v>2.21</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E43" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates with additional codes for figures
</commit_message>
<xml_diff>
--- a/3_intermediate/OR_import.xlsx
+++ b/3_intermediate/OR_import.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="70" documentId="11_88D1FD514068A76A5F098802EB9E65EADBDC33C4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED8ACDB4-862F-44AB-B542-04515194D176}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="5415" yWindow="1065" windowWidth="16140" windowHeight="14730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22905" windowHeight="11505"/>
   </bookViews>
   <sheets>
-    <sheet name="Table" sheetId="1" r:id="rId1"/>
+    <sheet name="Prov_5_inc" sheetId="3" r:id="rId1"/>
+    <sheet name="Prov_5" sheetId="2" r:id="rId2"/>
+    <sheet name="Table" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="37">
   <si>
     <t>OR</t>
   </si>
@@ -105,11 +106,38 @@
   <si>
     <t>Edu: Graduate (ref: &lt;High School)</t>
   </si>
+  <si>
+    <t>NFL &amp; NS</t>
+  </si>
+  <si>
+    <t>QC</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>MT &amp; AB</t>
+  </si>
+  <si>
+    <t>BC</t>
+  </si>
+  <si>
+    <t>U/R: Urban Others (ref: Rural)</t>
+  </si>
+  <si>
+    <t>Prov</t>
+  </si>
+  <si>
+    <t>Outbreak Peak*</t>
+  </si>
+  <si>
+    <t>Avg Incidence Rate 15 Days ago</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -424,11 +452,2469 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>1.07</v>
+      </c>
+      <c r="C2">
+        <v>0.94</v>
+      </c>
+      <c r="D2">
+        <v>1.21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.8</v>
+      </c>
+      <c r="D3">
+        <v>1.25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>1.49</v>
+      </c>
+      <c r="C4">
+        <v>0.96</v>
+      </c>
+      <c r="D4">
+        <v>2.33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <v>0.63</v>
+      </c>
+      <c r="C5">
+        <v>0.24</v>
+      </c>
+      <c r="D5">
+        <v>1.52</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>1.31</v>
+      </c>
+      <c r="C6">
+        <v>0.59</v>
+      </c>
+      <c r="D6">
+        <v>2.96</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>0.94</v>
+      </c>
+      <c r="C7">
+        <v>0.46</v>
+      </c>
+      <c r="D7">
+        <v>1.91</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="C8">
+        <v>0.54</v>
+      </c>
+      <c r="D8">
+        <v>2.29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>0.6</v>
+      </c>
+      <c r="C9">
+        <v>0.3</v>
+      </c>
+      <c r="D9">
+        <v>1.21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
+        <v>1.17</v>
+      </c>
+      <c r="C10">
+        <v>0.59</v>
+      </c>
+      <c r="D10">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11">
+        <v>1.06</v>
+      </c>
+      <c r="C11">
+        <v>0.53</v>
+      </c>
+      <c r="D11">
+        <v>2.09</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>0.99</v>
+      </c>
+      <c r="C13">
+        <v>0.97</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>1.21</v>
+      </c>
+      <c r="C14">
+        <v>0.95</v>
+      </c>
+      <c r="D14">
+        <v>1.55</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15">
+        <v>0.91</v>
+      </c>
+      <c r="C15">
+        <v>0.86</v>
+      </c>
+      <c r="D15">
+        <v>0.95</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="C16">
+        <v>0.95</v>
+      </c>
+      <c r="D16">
+        <v>1.3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>1.08</v>
+      </c>
+      <c r="C17">
+        <v>0.82</v>
+      </c>
+      <c r="D17">
+        <v>1.43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C18">
+        <v>0.04</v>
+      </c>
+      <c r="D18">
+        <v>0.11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19">
+        <v>0.97</v>
+      </c>
+      <c r="C19">
+        <v>0.54</v>
+      </c>
+      <c r="D19">
+        <v>1.75</v>
+      </c>
+      <c r="E19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20">
+        <v>0.34</v>
+      </c>
+      <c r="C20">
+        <v>0.11</v>
+      </c>
+      <c r="D20">
+        <v>0.94</v>
+      </c>
+      <c r="E20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>1.65</v>
+      </c>
+      <c r="C21">
+        <v>0.86</v>
+      </c>
+      <c r="D21">
+        <v>3.17</v>
+      </c>
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>1.77</v>
+      </c>
+      <c r="C22">
+        <v>0.88</v>
+      </c>
+      <c r="D22">
+        <v>3.59</v>
+      </c>
+      <c r="E22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>1.18</v>
+      </c>
+      <c r="C23">
+        <v>0.63</v>
+      </c>
+      <c r="D23">
+        <v>2.23</v>
+      </c>
+      <c r="E23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <v>0.99</v>
+      </c>
+      <c r="C24">
+        <v>0.54</v>
+      </c>
+      <c r="D24">
+        <v>1.84</v>
+      </c>
+      <c r="E24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
+        <v>0.72</v>
+      </c>
+      <c r="C25">
+        <v>0.39</v>
+      </c>
+      <c r="D25">
+        <v>1.37</v>
+      </c>
+      <c r="E25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>0.88</v>
+      </c>
+      <c r="C27">
+        <v>0.86</v>
+      </c>
+      <c r="D27">
+        <v>0.89</v>
+      </c>
+      <c r="E27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>0.25</v>
+      </c>
+      <c r="C28">
+        <v>0.19</v>
+      </c>
+      <c r="D28">
+        <v>0.33</v>
+      </c>
+      <c r="E28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29">
+        <v>1.05</v>
+      </c>
+      <c r="C29">
+        <v>1.02</v>
+      </c>
+      <c r="D29">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="E29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30">
+        <v>0.96</v>
+      </c>
+      <c r="C30">
+        <v>0.86</v>
+      </c>
+      <c r="D30">
+        <v>1.08</v>
+      </c>
+      <c r="E30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31">
+        <v>1.23</v>
+      </c>
+      <c r="C31">
+        <v>1.0001</v>
+      </c>
+      <c r="D31">
+        <v>1.52</v>
+      </c>
+      <c r="E31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <v>0.88</v>
+      </c>
+      <c r="C32">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D32">
+        <v>1.36</v>
+      </c>
+      <c r="E32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>0.99</v>
+      </c>
+      <c r="C33">
+        <v>0.6</v>
+      </c>
+      <c r="D33">
+        <v>1.64</v>
+      </c>
+      <c r="E33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34">
+        <v>0.9</v>
+      </c>
+      <c r="C34">
+        <v>0.5</v>
+      </c>
+      <c r="D34">
+        <v>1.65</v>
+      </c>
+      <c r="E34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35">
+        <v>0.81</v>
+      </c>
+      <c r="C35">
+        <v>0.42</v>
+      </c>
+      <c r="D35">
+        <v>1.53</v>
+      </c>
+      <c r="E35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36">
+        <v>0.62</v>
+      </c>
+      <c r="C36">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D36">
+        <v>1.33</v>
+      </c>
+      <c r="E36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37">
+        <v>0.71</v>
+      </c>
+      <c r="C37">
+        <v>0.37</v>
+      </c>
+      <c r="D37">
+        <v>1.3</v>
+      </c>
+      <c r="E37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38">
+        <v>0.86</v>
+      </c>
+      <c r="C38">
+        <v>0.46</v>
+      </c>
+      <c r="D38">
+        <v>1.57</v>
+      </c>
+      <c r="E38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39">
+        <v>0.81</v>
+      </c>
+      <c r="C39">
+        <v>0.43</v>
+      </c>
+      <c r="D39">
+        <v>1.48</v>
+      </c>
+      <c r="E39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41">
+        <v>0.98</v>
+      </c>
+      <c r="C41">
+        <v>0.97</v>
+      </c>
+      <c r="D41">
+        <v>0.99</v>
+      </c>
+      <c r="E41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42">
+        <v>0.92</v>
+      </c>
+      <c r="C42">
+        <v>0.73</v>
+      </c>
+      <c r="D42">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="E42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43">
+        <v>0.96</v>
+      </c>
+      <c r="C43">
+        <v>0.94</v>
+      </c>
+      <c r="D43">
+        <v>0.97</v>
+      </c>
+      <c r="E43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44">
+        <v>1.01</v>
+      </c>
+      <c r="C44">
+        <v>0.89</v>
+      </c>
+      <c r="D44">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E44" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45">
+        <v>1.21</v>
+      </c>
+      <c r="C45">
+        <v>0.97</v>
+      </c>
+      <c r="D45">
+        <v>1.51</v>
+      </c>
+      <c r="E45" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="C46">
+        <v>0.48</v>
+      </c>
+      <c r="D46">
+        <v>2.52</v>
+      </c>
+      <c r="E46" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47">
+        <v>0.46</v>
+      </c>
+      <c r="C47">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D47">
+        <v>1.41</v>
+      </c>
+      <c r="E47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D48">
+        <v>1.73</v>
+      </c>
+      <c r="E48" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49">
+        <v>1.93</v>
+      </c>
+      <c r="C49">
+        <v>1.0001</v>
+      </c>
+      <c r="D49">
+        <v>3.77</v>
+      </c>
+      <c r="E49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50">
+        <v>1.23</v>
+      </c>
+      <c r="C50">
+        <v>0.59</v>
+      </c>
+      <c r="D50">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="E50" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51">
+        <v>1.08</v>
+      </c>
+      <c r="C51">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D51">
+        <v>2.11</v>
+      </c>
+      <c r="E51" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52">
+        <v>2.09</v>
+      </c>
+      <c r="C52">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="D52">
+        <v>3.95</v>
+      </c>
+      <c r="E52" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53">
+        <v>1.42</v>
+      </c>
+      <c r="C53">
+        <v>0.75</v>
+      </c>
+      <c r="D53">
+        <v>2.74</v>
+      </c>
+      <c r="E53" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55">
+        <v>1.02</v>
+      </c>
+      <c r="C55">
+        <v>1.0001</v>
+      </c>
+      <c r="D55">
+        <v>1.03</v>
+      </c>
+      <c r="E55" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56">
+        <v>0.95</v>
+      </c>
+      <c r="C56">
+        <v>0.76</v>
+      </c>
+      <c r="D56">
+        <v>1.2</v>
+      </c>
+      <c r="E56" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57">
+        <v>0.99</v>
+      </c>
+      <c r="C57">
+        <v>0.98</v>
+      </c>
+      <c r="D57">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="E57" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="C58">
+        <v>0.99</v>
+      </c>
+      <c r="D58">
+        <v>1.29</v>
+      </c>
+      <c r="E58" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59">
+        <v>0.99</v>
+      </c>
+      <c r="C59">
+        <v>0.78</v>
+      </c>
+      <c r="D59">
+        <v>1.26</v>
+      </c>
+      <c r="E59" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60">
+        <v>0.26</v>
+      </c>
+      <c r="C60">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D60">
+        <v>0.48</v>
+      </c>
+      <c r="E60" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>33</v>
+      </c>
+      <c r="B61">
+        <v>0.26</v>
+      </c>
+      <c r="C61">
+        <v>0.12</v>
+      </c>
+      <c r="D61">
+        <v>0.54</v>
+      </c>
+      <c r="E61" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>11</v>
+      </c>
+      <c r="B62">
+        <v>0.5</v>
+      </c>
+      <c r="C62">
+        <v>0.26</v>
+      </c>
+      <c r="D62">
+        <v>0.9</v>
+      </c>
+      <c r="E62" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>23</v>
+      </c>
+      <c r="B63">
+        <v>2.77</v>
+      </c>
+      <c r="C63">
+        <v>1.35</v>
+      </c>
+      <c r="D63">
+        <v>5.91</v>
+      </c>
+      <c r="E63" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>24</v>
+      </c>
+      <c r="B64">
+        <v>0.65</v>
+      </c>
+      <c r="C64">
+        <v>0.27</v>
+      </c>
+      <c r="D64">
+        <v>1.57</v>
+      </c>
+      <c r="E64" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>25</v>
+      </c>
+      <c r="B65">
+        <v>1.56</v>
+      </c>
+      <c r="C65">
+        <v>0.77</v>
+      </c>
+      <c r="D65">
+        <v>3.27</v>
+      </c>
+      <c r="E65" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>26</v>
+      </c>
+      <c r="B66">
+        <v>1.69</v>
+      </c>
+      <c r="C66">
+        <v>0.85</v>
+      </c>
+      <c r="D66">
+        <v>3.52</v>
+      </c>
+      <c r="E66" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>27</v>
+      </c>
+      <c r="B67">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="C67">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D67">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="E67" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>8</v>
+      </c>
+      <c r="B69">
+        <v>0.93</v>
+      </c>
+      <c r="C69">
+        <v>0.92</v>
+      </c>
+      <c r="D69">
+        <v>0.95</v>
+      </c>
+      <c r="E69" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C70">
+        <v>0.43</v>
+      </c>
+      <c r="D70">
+        <v>0.7</v>
+      </c>
+      <c r="E70" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B71">
+        <v>0.87</v>
+      </c>
+      <c r="C71">
+        <v>0.84</v>
+      </c>
+      <c r="D71">
+        <v>0.89</v>
+      </c>
+      <c r="E71" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E71"/>
+  <sheetViews>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection sqref="A1:E71"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="3" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="C2">
+        <v>0.95</v>
+      </c>
+      <c r="D2">
+        <v>1.25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>1.06</v>
+      </c>
+      <c r="C3">
+        <v>0.83</v>
+      </c>
+      <c r="D3">
+        <v>1.35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>1.28</v>
+      </c>
+      <c r="C4">
+        <v>0.81</v>
+      </c>
+      <c r="D4">
+        <v>2.04</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C5">
+        <v>0.2</v>
+      </c>
+      <c r="D5">
+        <v>1.4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>1.35</v>
+      </c>
+      <c r="C6">
+        <v>0.53</v>
+      </c>
+      <c r="D6">
+        <v>3.65</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>0.95</v>
+      </c>
+      <c r="C7">
+        <v>0.45</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>1.3</v>
+      </c>
+      <c r="C8">
+        <v>0.61</v>
+      </c>
+      <c r="D8">
+        <v>2.78</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>0.77</v>
+      </c>
+      <c r="C9">
+        <v>0.37</v>
+      </c>
+      <c r="D9">
+        <v>1.6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
+        <v>1.25</v>
+      </c>
+      <c r="C10">
+        <v>0.61</v>
+      </c>
+      <c r="D10">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="C11">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D11">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0.98</v>
+      </c>
+      <c r="D12">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>0.98</v>
+      </c>
+      <c r="C13">
+        <v>0.97</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>1.07</v>
+      </c>
+      <c r="C14">
+        <v>0.83</v>
+      </c>
+      <c r="D14">
+        <v>1.37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C15">
+        <v>0.34</v>
+      </c>
+      <c r="D15">
+        <v>0.86</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="C16">
+        <v>0.92</v>
+      </c>
+      <c r="D16">
+        <v>1.29</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="C17">
+        <v>0.84</v>
+      </c>
+      <c r="D17">
+        <v>1.53</v>
+      </c>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>0.06</v>
+      </c>
+      <c r="C18">
+        <v>0.04</v>
+      </c>
+      <c r="D18">
+        <v>0.11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19">
+        <v>0.73</v>
+      </c>
+      <c r="C19">
+        <v>0.37</v>
+      </c>
+      <c r="D19">
+        <v>1.4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20">
+        <v>0.43</v>
+      </c>
+      <c r="C20">
+        <v>0.13</v>
+      </c>
+      <c r="D20">
+        <v>1.25</v>
+      </c>
+      <c r="E20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>1.51</v>
+      </c>
+      <c r="C21">
+        <v>0.76</v>
+      </c>
+      <c r="D21">
+        <v>3.04</v>
+      </c>
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>1.89</v>
+      </c>
+      <c r="C22">
+        <v>0.88</v>
+      </c>
+      <c r="D22">
+        <v>4.09</v>
+      </c>
+      <c r="E22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="C23">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D23">
+        <v>2.25</v>
+      </c>
+      <c r="E23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <v>0.92</v>
+      </c>
+      <c r="C24">
+        <v>0.48</v>
+      </c>
+      <c r="D24">
+        <v>1.78</v>
+      </c>
+      <c r="E24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
+        <v>0.71</v>
+      </c>
+      <c r="C25">
+        <v>0.37</v>
+      </c>
+      <c r="D25">
+        <v>1.41</v>
+      </c>
+      <c r="E25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>0.96</v>
+      </c>
+      <c r="C26">
+        <v>0.93</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>0.87</v>
+      </c>
+      <c r="C27">
+        <v>0.85</v>
+      </c>
+      <c r="D27">
+        <v>0.89</v>
+      </c>
+      <c r="E27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>0.24</v>
+      </c>
+      <c r="C28">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D28">
+        <v>0.33</v>
+      </c>
+      <c r="E28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29">
+        <v>31.8</v>
+      </c>
+      <c r="C29">
+        <v>6.6</v>
+      </c>
+      <c r="D29">
+        <v>572</v>
+      </c>
+      <c r="E29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30">
+        <v>0.96</v>
+      </c>
+      <c r="C30">
+        <v>0.85</v>
+      </c>
+      <c r="D30">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="E30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31">
+        <v>1.2</v>
+      </c>
+      <c r="C31">
+        <v>0.96</v>
+      </c>
+      <c r="D31">
+        <v>1.51</v>
+      </c>
+      <c r="E31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <v>0.94</v>
+      </c>
+      <c r="C32">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D32">
+        <v>1.5</v>
+      </c>
+      <c r="E32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>1.2</v>
+      </c>
+      <c r="C33">
+        <v>0.7</v>
+      </c>
+      <c r="D33">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="E33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34">
+        <v>0.98</v>
+      </c>
+      <c r="C34">
+        <v>0.52</v>
+      </c>
+      <c r="D34">
+        <v>1.88</v>
+      </c>
+      <c r="E34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35">
+        <v>0.83</v>
+      </c>
+      <c r="C35">
+        <v>0.41</v>
+      </c>
+      <c r="D35">
+        <v>1.61</v>
+      </c>
+      <c r="E35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36">
+        <v>0.6</v>
+      </c>
+      <c r="C36">
+        <v>0.26</v>
+      </c>
+      <c r="D36">
+        <v>1.34</v>
+      </c>
+      <c r="E36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37">
+        <v>0.6</v>
+      </c>
+      <c r="C37">
+        <v>0.3</v>
+      </c>
+      <c r="D37">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="E37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38">
+        <v>0.8</v>
+      </c>
+      <c r="C38">
+        <v>0.41</v>
+      </c>
+      <c r="D38">
+        <v>1.5</v>
+      </c>
+      <c r="E38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39">
+        <v>0.68</v>
+      </c>
+      <c r="C39">
+        <v>0.35</v>
+      </c>
+      <c r="D39">
+        <v>1.29</v>
+      </c>
+      <c r="E39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40">
+        <v>0.99</v>
+      </c>
+      <c r="C40">
+        <v>0.97</v>
+      </c>
+      <c r="D40">
+        <v>1.01</v>
+      </c>
+      <c r="E40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41">
+        <v>0.98</v>
+      </c>
+      <c r="C41">
+        <v>0.97</v>
+      </c>
+      <c r="D41">
+        <v>0.99</v>
+      </c>
+      <c r="E41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42">
+        <v>0.71</v>
+      </c>
+      <c r="C42">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D42">
+        <v>0.89</v>
+      </c>
+      <c r="E42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43">
+        <v>10.9</v>
+      </c>
+      <c r="C43">
+        <v>3.72</v>
+      </c>
+      <c r="D43">
+        <v>46.7</v>
+      </c>
+      <c r="E43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44">
+        <v>1.08</v>
+      </c>
+      <c r="C44">
+        <v>0.94</v>
+      </c>
+      <c r="D44">
+        <v>1.23</v>
+      </c>
+      <c r="E44" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45">
+        <v>1.18</v>
+      </c>
+      <c r="C45">
+        <v>0.93</v>
+      </c>
+      <c r="D45">
+        <v>1.51</v>
+      </c>
+      <c r="E45" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46">
+        <v>1.39</v>
+      </c>
+      <c r="C46">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D46">
+        <v>3.54</v>
+      </c>
+      <c r="E46" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C47">
+        <v>0.16</v>
+      </c>
+      <c r="D47">
+        <v>1.88</v>
+      </c>
+      <c r="E47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48">
+        <v>0.96</v>
+      </c>
+      <c r="C48">
+        <v>0.52</v>
+      </c>
+      <c r="D48">
+        <v>1.78</v>
+      </c>
+      <c r="E48" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C49">
+        <v>1.08</v>
+      </c>
+      <c r="D49">
+        <v>4.53</v>
+      </c>
+      <c r="E49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50">
+        <v>1.3</v>
+      </c>
+      <c r="C50">
+        <v>0.59</v>
+      </c>
+      <c r="D50">
+        <v>2.89</v>
+      </c>
+      <c r="E50" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="C51">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D51">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E51" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52">
+        <v>2.41</v>
+      </c>
+      <c r="C52">
+        <v>1.22</v>
+      </c>
+      <c r="D52">
+        <v>4.83</v>
+      </c>
+      <c r="E52" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53">
+        <v>1.55</v>
+      </c>
+      <c r="C53">
+        <v>0.78</v>
+      </c>
+      <c r="D53">
+        <v>3.15</v>
+      </c>
+      <c r="E53" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>0.98</v>
+      </c>
+      <c r="D54">
+        <v>1.03</v>
+      </c>
+      <c r="E54" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55">
+        <v>1.02</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>1.04</v>
+      </c>
+      <c r="E55" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56">
+        <v>0.93</v>
+      </c>
+      <c r="C56">
+        <v>0.73</v>
+      </c>
+      <c r="D56">
+        <v>1.19</v>
+      </c>
+      <c r="E56" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>35</v>
+      </c>
+      <c r="B57">
+        <v>1.54</v>
+      </c>
+      <c r="C57">
+        <v>0.87</v>
+      </c>
+      <c r="D57">
+        <v>2.75</v>
+      </c>
+      <c r="E57" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="C58">
+        <v>0.95</v>
+      </c>
+      <c r="D58">
+        <v>1.24</v>
+      </c>
+      <c r="E58" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59">
+        <v>1.04</v>
+      </c>
+      <c r="C59">
+        <v>0.81</v>
+      </c>
+      <c r="D59">
+        <v>1.32</v>
+      </c>
+      <c r="E59" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C60">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D60">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E60" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>33</v>
+      </c>
+      <c r="B61">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C61">
+        <v>0.13</v>
+      </c>
+      <c r="D61">
+        <v>0.6</v>
+      </c>
+      <c r="E61" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>11</v>
+      </c>
+      <c r="B62">
+        <v>0.51</v>
+      </c>
+      <c r="C62">
+        <v>0.27</v>
+      </c>
+      <c r="D62">
+        <v>0.95</v>
+      </c>
+      <c r="E62" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>23</v>
+      </c>
+      <c r="B63">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="C63">
+        <v>1.22</v>
+      </c>
+      <c r="D63">
+        <v>5.28</v>
+      </c>
+      <c r="E63" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>24</v>
+      </c>
+      <c r="B64">
+        <v>0.67</v>
+      </c>
+      <c r="C64">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D64">
+        <v>1.64</v>
+      </c>
+      <c r="E64" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>25</v>
+      </c>
+      <c r="B65">
+        <v>1.46</v>
+      </c>
+      <c r="C65">
+        <v>0.72</v>
+      </c>
+      <c r="D65">
+        <v>3.05</v>
+      </c>
+      <c r="E65" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>26</v>
+      </c>
+      <c r="B66">
+        <v>1.56</v>
+      </c>
+      <c r="C66">
+        <v>0.78</v>
+      </c>
+      <c r="D66">
+        <v>3.24</v>
+      </c>
+      <c r="E66" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>27</v>
+      </c>
+      <c r="B67">
+        <v>2.11</v>
+      </c>
+      <c r="C67">
+        <v>1.06</v>
+      </c>
+      <c r="D67">
+        <v>4.38</v>
+      </c>
+      <c r="E67" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68">
+        <v>0.99</v>
+      </c>
+      <c r="C68">
+        <v>0.96</v>
+      </c>
+      <c r="D68">
+        <v>1.01</v>
+      </c>
+      <c r="E68" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>8</v>
+      </c>
+      <c r="B69">
+        <v>0.94</v>
+      </c>
+      <c r="C69">
+        <v>0.92</v>
+      </c>
+      <c r="D69">
+        <v>0.95</v>
+      </c>
+      <c r="E69" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70">
+        <v>0.54</v>
+      </c>
+      <c r="C70">
+        <v>0.42</v>
+      </c>
+      <c r="D70">
+        <v>0.69</v>
+      </c>
+      <c r="E70" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B71">
+        <v>0.72</v>
+      </c>
+      <c r="C71">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D71">
+        <v>1.89</v>
+      </c>
+      <c r="E71" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection sqref="A1:E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated fig, finished letter & supplement
</commit_message>
<xml_diff>
--- a/3_intermediate/OR_import.xlsx
+++ b/3_intermediate/OR_import.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22905" windowHeight="11505" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22905" windowHeight="11505"/>
   </bookViews>
   <sheets>
     <sheet name="Prov_5_inc" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="35">
   <si>
     <t>OR</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Traveling Distance (per 25km)</t>
+  </si>
+  <si>
+    <t>NL &amp; NS</t>
   </si>
 </sst>
 </file>
@@ -449,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,16 +487,16 @@
         <v>13</v>
       </c>
       <c r="B2">
-        <v>1.07</v>
+        <v>1.06</v>
       </c>
       <c r="C2">
-        <v>0.94</v>
+        <v>0.92</v>
       </c>
       <c r="D2">
         <v>1.21</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -501,16 +504,16 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="C3">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="D3">
-        <v>1.25</v>
+        <v>1.39</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -518,16 +521,16 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <v>1.49</v>
+        <v>1.28</v>
       </c>
       <c r="C4">
-        <v>0.96</v>
+        <v>0.81</v>
       </c>
       <c r="D4">
-        <v>2.33</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -535,16 +538,16 @@
         <v>28</v>
       </c>
       <c r="B5">
-        <v>0.63</v>
+        <v>0.54</v>
       </c>
       <c r="C5">
-        <v>0.24</v>
+        <v>0.19</v>
       </c>
       <c r="D5">
-        <v>1.52</v>
+        <v>1.38</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -552,16 +555,16 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>1.31</v>
+        <v>1.37</v>
       </c>
       <c r="C6">
-        <v>0.59</v>
+        <v>0.53</v>
       </c>
       <c r="D6">
-        <v>2.96</v>
+        <v>3.67</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -569,16 +572,16 @@
         <v>18</v>
       </c>
       <c r="B7">
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="C7">
-        <v>0.46</v>
+        <v>0.42</v>
       </c>
       <c r="D7">
-        <v>1.91</v>
+        <v>1.89</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -586,16 +589,16 @@
         <v>19</v>
       </c>
       <c r="B8">
-        <v>1.1200000000000001</v>
+        <v>1.17</v>
       </c>
       <c r="C8">
         <v>0.54</v>
       </c>
       <c r="D8">
-        <v>2.29</v>
+        <v>2.5</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -603,16 +606,16 @@
         <v>20</v>
       </c>
       <c r="B9">
-        <v>0.6</v>
+        <v>0.69</v>
       </c>
       <c r="C9">
-        <v>0.3</v>
+        <v>0.33</v>
       </c>
       <c r="D9">
-        <v>1.21</v>
+        <v>1.45</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -620,16 +623,16 @@
         <v>21</v>
       </c>
       <c r="B10">
-        <v>1.17</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="C10">
-        <v>0.59</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="D10">
-        <v>2.2999999999999998</v>
+        <v>2.37</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -637,16 +640,16 @@
         <v>22</v>
       </c>
       <c r="B11">
-        <v>1.06</v>
+        <v>1.03</v>
       </c>
       <c r="C11">
-        <v>0.53</v>
+        <v>0.5</v>
       </c>
       <c r="D11">
-        <v>2.09</v>
+        <v>2.12</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -654,33 +657,33 @@
         <v>5</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>1.01</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>1.03</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B13">
-        <v>0.99</v>
+        <v>0.68</v>
       </c>
       <c r="C13">
+        <v>0.48</v>
+      </c>
+      <c r="D13">
         <v>0.97</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -688,16 +691,16 @@
         <v>6</v>
       </c>
       <c r="B14">
-        <v>1.21</v>
+        <v>1.39</v>
       </c>
       <c r="C14">
-        <v>0.95</v>
+        <v>1.06</v>
       </c>
       <c r="D14">
-        <v>1.55</v>
+        <v>1.82</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -705,16 +708,16 @@
         <v>31</v>
       </c>
       <c r="B15">
-        <v>0.91</v>
+        <v>0.38</v>
       </c>
       <c r="C15">
-        <v>0.86</v>
+        <v>0.22</v>
       </c>
       <c r="D15">
-        <v>0.95</v>
+        <v>0.63</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -722,13 +725,13 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>1.1100000000000001</v>
+        <v>1.08</v>
       </c>
       <c r="C16">
-        <v>0.95</v>
+        <v>0.91</v>
       </c>
       <c r="D16">
-        <v>1.3</v>
+        <v>1.28</v>
       </c>
       <c r="E16" t="s">
         <v>24</v>
@@ -739,13 +742,13 @@
         <v>12</v>
       </c>
       <c r="B17">
-        <v>1.08</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="C17">
-        <v>0.82</v>
+        <v>0.81</v>
       </c>
       <c r="D17">
-        <v>1.43</v>
+        <v>1.47</v>
       </c>
       <c r="E17" t="s">
         <v>24</v>
@@ -756,13 +759,13 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="C18">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="D18">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="E18" t="s">
         <v>24</v>
@@ -773,13 +776,13 @@
         <v>28</v>
       </c>
       <c r="B19">
-        <v>0.97</v>
+        <v>0.75</v>
       </c>
       <c r="C19">
-        <v>0.54</v>
+        <v>0.39</v>
       </c>
       <c r="D19">
-        <v>1.75</v>
+        <v>1.42</v>
       </c>
       <c r="E19" t="s">
         <v>24</v>
@@ -790,13 +793,13 @@
         <v>10</v>
       </c>
       <c r="B20">
-        <v>0.34</v>
+        <v>0.45</v>
       </c>
       <c r="C20">
-        <v>0.11</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D20">
-        <v>0.94</v>
+        <v>1.32</v>
       </c>
       <c r="E20" t="s">
         <v>24</v>
@@ -807,13 +810,13 @@
         <v>18</v>
       </c>
       <c r="B21">
-        <v>1.65</v>
+        <v>1.58</v>
       </c>
       <c r="C21">
-        <v>0.86</v>
+        <v>0.8</v>
       </c>
       <c r="D21">
-        <v>3.17</v>
+        <v>3.12</v>
       </c>
       <c r="E21" t="s">
         <v>24</v>
@@ -824,13 +827,13 @@
         <v>19</v>
       </c>
       <c r="B22">
-        <v>1.77</v>
+        <v>1.98</v>
       </c>
       <c r="C22">
-        <v>0.88</v>
+        <v>0.94</v>
       </c>
       <c r="D22">
-        <v>3.59</v>
+        <v>4.22</v>
       </c>
       <c r="E22" t="s">
         <v>24</v>
@@ -841,10 +844,10 @@
         <v>20</v>
       </c>
       <c r="B23">
-        <v>1.18</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C23">
-        <v>0.63</v>
+        <v>0.6</v>
       </c>
       <c r="D23">
         <v>2.23</v>
@@ -858,13 +861,13 @@
         <v>21</v>
       </c>
       <c r="B24">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="C24">
-        <v>0.54</v>
+        <v>0.5</v>
       </c>
       <c r="D24">
-        <v>1.84</v>
+        <v>1.81</v>
       </c>
       <c r="E24" t="s">
         <v>24</v>
@@ -875,13 +878,13 @@
         <v>22</v>
       </c>
       <c r="B25">
-        <v>0.72</v>
+        <v>0.77</v>
       </c>
       <c r="C25">
-        <v>0.39</v>
+        <v>0.4</v>
       </c>
       <c r="D25">
-        <v>1.37</v>
+        <v>1.5</v>
       </c>
       <c r="E25" t="s">
         <v>24</v>
@@ -892,13 +895,13 @@
         <v>5</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>0.96</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0.93</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="E26" t="s">
         <v>24</v>
@@ -906,16 +909,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B27">
-        <v>0.88</v>
+        <v>0.03</v>
       </c>
       <c r="C27">
-        <v>0.86</v>
+        <v>0.02</v>
       </c>
       <c r="D27">
-        <v>0.89</v>
+        <v>0.06</v>
       </c>
       <c r="E27" t="s">
         <v>24</v>
@@ -926,10 +929,10 @@
         <v>6</v>
       </c>
       <c r="B28">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="C28">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
       <c r="D28">
         <v>0.33</v>
@@ -943,13 +946,13 @@
         <v>31</v>
       </c>
       <c r="B29">
-        <v>1.05</v>
+        <v>1.43</v>
       </c>
       <c r="C29">
-        <v>1.02</v>
+        <v>0.99</v>
       </c>
       <c r="D29">
-        <v>1.0900000000000001</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="E29" t="s">
         <v>24</v>
@@ -960,13 +963,13 @@
         <v>13</v>
       </c>
       <c r="B30">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="C30">
-        <v>0.86</v>
+        <v>0.84</v>
       </c>
       <c r="D30">
-        <v>1.08</v>
+        <v>1.07</v>
       </c>
       <c r="E30" t="s">
         <v>25</v>
@@ -980,10 +983,10 @@
         <v>1.23</v>
       </c>
       <c r="C31">
-        <v>1.0001</v>
+        <v>0.98</v>
       </c>
       <c r="D31">
-        <v>1.52</v>
+        <v>1.55</v>
       </c>
       <c r="E31" t="s">
         <v>25</v>
@@ -994,13 +997,13 @@
         <v>17</v>
       </c>
       <c r="B32">
-        <v>0.88</v>
+        <v>0.9</v>
       </c>
       <c r="C32">
         <v>0.56000000000000005</v>
       </c>
       <c r="D32">
-        <v>1.36</v>
+        <v>1.44</v>
       </c>
       <c r="E32" t="s">
         <v>25</v>
@@ -1011,13 +1014,13 @@
         <v>28</v>
       </c>
       <c r="B33">
-        <v>0.99</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C33">
-        <v>0.6</v>
+        <v>0.67</v>
       </c>
       <c r="D33">
-        <v>1.64</v>
+        <v>1.97</v>
       </c>
       <c r="E33" t="s">
         <v>25</v>
@@ -1028,13 +1031,13 @@
         <v>10</v>
       </c>
       <c r="B34">
-        <v>0.9</v>
+        <v>0.99</v>
       </c>
       <c r="C34">
-        <v>0.5</v>
+        <v>0.52</v>
       </c>
       <c r="D34">
-        <v>1.65</v>
+        <v>1.9</v>
       </c>
       <c r="E34" t="s">
         <v>25</v>
@@ -1045,13 +1048,13 @@
         <v>18</v>
       </c>
       <c r="B35">
-        <v>0.81</v>
+        <v>0.78</v>
       </c>
       <c r="C35">
-        <v>0.42</v>
+        <v>0.39</v>
       </c>
       <c r="D35">
-        <v>1.53</v>
+        <v>1.52</v>
       </c>
       <c r="E35" t="s">
         <v>25</v>
@@ -1062,13 +1065,13 @@
         <v>19</v>
       </c>
       <c r="B36">
-        <v>0.62</v>
+        <v>0.63</v>
       </c>
       <c r="C36">
         <v>0.28000000000000003</v>
       </c>
       <c r="D36">
-        <v>1.33</v>
+        <v>1.43</v>
       </c>
       <c r="E36" t="s">
         <v>25</v>
@@ -1079,13 +1082,13 @@
         <v>20</v>
       </c>
       <c r="B37">
-        <v>0.71</v>
+        <v>0.6</v>
       </c>
       <c r="C37">
-        <v>0.37</v>
+        <v>0.31</v>
       </c>
       <c r="D37">
-        <v>1.3</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="E37" t="s">
         <v>25</v>
@@ -1096,13 +1099,13 @@
         <v>21</v>
       </c>
       <c r="B38">
-        <v>0.86</v>
+        <v>0.82</v>
       </c>
       <c r="C38">
-        <v>0.46</v>
+        <v>0.42</v>
       </c>
       <c r="D38">
-        <v>1.57</v>
+        <v>1.55</v>
       </c>
       <c r="E38" t="s">
         <v>25</v>
@@ -1113,13 +1116,13 @@
         <v>22</v>
       </c>
       <c r="B39">
-        <v>0.81</v>
+        <v>0.71</v>
       </c>
       <c r="C39">
-        <v>0.43</v>
+        <v>0.36</v>
       </c>
       <c r="D39">
-        <v>1.48</v>
+        <v>1.34</v>
       </c>
       <c r="E39" t="s">
         <v>25</v>
@@ -1130,13 +1133,13 @@
         <v>5</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>0.96</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>1.01</v>
       </c>
       <c r="E40" t="s">
         <v>25</v>
@@ -1144,16 +1147,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B41">
-        <v>0.98</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="C41">
-        <v>0.97</v>
+        <v>0.41</v>
       </c>
       <c r="D41">
-        <v>0.99</v>
+        <v>0.77</v>
       </c>
       <c r="E41" t="s">
         <v>25</v>
@@ -1164,13 +1167,13 @@
         <v>6</v>
       </c>
       <c r="B42">
-        <v>0.92</v>
+        <v>0.98</v>
       </c>
       <c r="C42">
-        <v>0.73</v>
+        <v>0.77</v>
       </c>
       <c r="D42">
-        <v>1.1599999999999999</v>
+        <v>1.27</v>
       </c>
       <c r="E42" t="s">
         <v>25</v>
@@ -1181,13 +1184,13 @@
         <v>31</v>
       </c>
       <c r="B43">
-        <v>0.96</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="C43">
-        <v>0.94</v>
+        <v>0.49</v>
       </c>
       <c r="D43">
-        <v>0.97</v>
+        <v>0.69</v>
       </c>
       <c r="E43" t="s">
         <v>25</v>
@@ -1198,13 +1201,13 @@
         <v>13</v>
       </c>
       <c r="B44">
-        <v>1.01</v>
+        <v>1.08</v>
       </c>
       <c r="C44">
-        <v>0.89</v>
+        <v>0.94</v>
       </c>
       <c r="D44">
-        <v>1.1499999999999999</v>
+        <v>1.23</v>
       </c>
       <c r="E44" t="s">
         <v>26</v>
@@ -1215,10 +1218,10 @@
         <v>12</v>
       </c>
       <c r="B45">
-        <v>1.21</v>
+        <v>1.19</v>
       </c>
       <c r="C45">
-        <v>0.97</v>
+        <v>0.93</v>
       </c>
       <c r="D45">
         <v>1.51</v>
@@ -1232,13 +1235,13 @@
         <v>17</v>
       </c>
       <c r="B46">
-        <v>1.1100000000000001</v>
+        <v>1.35</v>
       </c>
       <c r="C46">
-        <v>0.48</v>
+        <v>0.53</v>
       </c>
       <c r="D46">
-        <v>2.52</v>
+        <v>3.43</v>
       </c>
       <c r="E46" t="s">
         <v>26</v>
@@ -1249,13 +1252,13 @@
         <v>28</v>
       </c>
       <c r="B47">
-        <v>0.46</v>
+        <v>0.54</v>
       </c>
       <c r="C47">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="D47">
-        <v>1.41</v>
+        <v>1.8</v>
       </c>
       <c r="E47" t="s">
         <v>26</v>
@@ -1266,13 +1269,13 @@
         <v>10</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>0.94</v>
       </c>
       <c r="C48">
-        <v>0.57999999999999996</v>
+        <v>0.51</v>
       </c>
       <c r="D48">
-        <v>1.73</v>
+        <v>1.75</v>
       </c>
       <c r="E48" t="s">
         <v>26</v>
@@ -1283,13 +1286,13 @@
         <v>18</v>
       </c>
       <c r="B49">
-        <v>1.93</v>
+        <v>2.17</v>
       </c>
       <c r="C49">
-        <v>1.0001</v>
+        <v>1.07</v>
       </c>
       <c r="D49">
-        <v>3.77</v>
+        <v>4.47</v>
       </c>
       <c r="E49" t="s">
         <v>26</v>
@@ -1300,13 +1303,13 @@
         <v>19</v>
       </c>
       <c r="B50">
-        <v>1.23</v>
+        <v>1.28</v>
       </c>
       <c r="C50">
-        <v>0.59</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="D50">
-        <v>2.5499999999999998</v>
+        <v>2.83</v>
       </c>
       <c r="E50" t="s">
         <v>26</v>
@@ -1317,13 +1320,13 @@
         <v>20</v>
       </c>
       <c r="B51">
-        <v>1.08</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C51">
-        <v>0.56000000000000005</v>
+        <v>0.54</v>
       </c>
       <c r="D51">
-        <v>2.11</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="E51" t="s">
         <v>26</v>
@@ -1334,13 +1337,13 @@
         <v>21</v>
       </c>
       <c r="B52">
-        <v>2.09</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="C52">
-        <v>1.1100000000000001</v>
+        <v>1.23</v>
       </c>
       <c r="D52">
-        <v>3.95</v>
+        <v>4.87</v>
       </c>
       <c r="E52" t="s">
         <v>26</v>
@@ -1351,13 +1354,13 @@
         <v>22</v>
       </c>
       <c r="B53">
-        <v>1.42</v>
+        <v>1.55</v>
       </c>
       <c r="C53">
-        <v>0.75</v>
+        <v>0.77</v>
       </c>
       <c r="D53">
-        <v>2.74</v>
+        <v>3.14</v>
       </c>
       <c r="E53" t="s">
         <v>26</v>
@@ -1371,10 +1374,10 @@
         <v>1</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>1.03</v>
       </c>
       <c r="E54" t="s">
         <v>26</v>
@@ -1382,16 +1385,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B55">
-        <v>1.02</v>
+        <v>1.65</v>
       </c>
       <c r="C55">
-        <v>1.0001</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="D55">
-        <v>1.03</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="E55" t="s">
         <v>26</v>
@@ -1402,10 +1405,10 @@
         <v>6</v>
       </c>
       <c r="B56">
-        <v>0.95</v>
+        <v>0.94</v>
       </c>
       <c r="C56">
-        <v>0.76</v>
+        <v>0.74</v>
       </c>
       <c r="D56">
         <v>1.2</v>
@@ -1419,13 +1422,13 @@
         <v>31</v>
       </c>
       <c r="B57">
+        <v>0.88</v>
+      </c>
+      <c r="C57">
+        <v>0.79</v>
+      </c>
+      <c r="D57">
         <v>0.99</v>
-      </c>
-      <c r="C57">
-        <v>0.98</v>
-      </c>
-      <c r="D57">
-        <v>0.99990000000000001</v>
       </c>
       <c r="E57" t="s">
         <v>26</v>
@@ -1436,13 +1439,13 @@
         <v>13</v>
       </c>
       <c r="B58">
-        <v>1.1299999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="C58">
         <v>0.99</v>
       </c>
       <c r="D58">
-        <v>1.29</v>
+        <v>1.32</v>
       </c>
       <c r="E58" t="s">
         <v>27</v>
@@ -1453,13 +1456,13 @@
         <v>12</v>
       </c>
       <c r="B59">
-        <v>0.99</v>
+        <v>1.01</v>
       </c>
       <c r="C59">
         <v>0.78</v>
       </c>
       <c r="D59">
-        <v>1.26</v>
+        <v>1.32</v>
       </c>
       <c r="E59" t="s">
         <v>27</v>
@@ -1470,13 +1473,13 @@
         <v>17</v>
       </c>
       <c r="B60">
-        <v>0.26</v>
+        <v>0.27</v>
       </c>
       <c r="C60">
-        <v>0.14000000000000001</v>
+        <v>0.13</v>
       </c>
       <c r="D60">
-        <v>0.48</v>
+        <v>0.54</v>
       </c>
       <c r="E60" t="s">
         <v>27</v>
@@ -1487,13 +1490,13 @@
         <v>28</v>
       </c>
       <c r="B61">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
       <c r="C61">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="D61">
-        <v>0.54</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="E61" t="s">
         <v>27</v>
@@ -1504,13 +1507,13 @@
         <v>10</v>
       </c>
       <c r="B62">
-        <v>0.5</v>
+        <v>0.59</v>
       </c>
       <c r="C62">
-        <v>0.26</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D62">
-        <v>0.9</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="E62" t="s">
         <v>27</v>
@@ -1521,13 +1524,13 @@
         <v>18</v>
       </c>
       <c r="B63">
-        <v>2.77</v>
+        <v>2.87</v>
       </c>
       <c r="C63">
         <v>1.35</v>
       </c>
       <c r="D63">
-        <v>5.91</v>
+        <v>6.36</v>
       </c>
       <c r="E63" t="s">
         <v>27</v>
@@ -1538,13 +1541,13 @@
         <v>19</v>
       </c>
       <c r="B64">
-        <v>0.65</v>
+        <v>0.64</v>
       </c>
       <c r="C64">
-        <v>0.27</v>
+        <v>0.25</v>
       </c>
       <c r="D64">
-        <v>1.57</v>
+        <v>1.63</v>
       </c>
       <c r="E64" t="s">
         <v>27</v>
@@ -1555,13 +1558,13 @@
         <v>20</v>
       </c>
       <c r="B65">
-        <v>1.56</v>
+        <v>1.63</v>
       </c>
       <c r="C65">
-        <v>0.77</v>
+        <v>0.78</v>
       </c>
       <c r="D65">
-        <v>3.27</v>
+        <v>3.54</v>
       </c>
       <c r="E65" t="s">
         <v>27</v>
@@ -1572,13 +1575,13 @@
         <v>21</v>
       </c>
       <c r="B66">
-        <v>1.69</v>
+        <v>1.84</v>
       </c>
       <c r="C66">
-        <v>0.85</v>
+        <v>0.89</v>
       </c>
       <c r="D66">
-        <v>3.52</v>
+        <v>3.97</v>
       </c>
       <c r="E66" t="s">
         <v>27</v>
@@ -1589,13 +1592,13 @@
         <v>22</v>
       </c>
       <c r="B67">
-        <v>2.2599999999999998</v>
+        <v>2.42</v>
       </c>
       <c r="C67">
-        <v>1.1299999999999999</v>
+        <v>1.17</v>
       </c>
       <c r="D67">
-        <v>4.6900000000000004</v>
+        <v>5.21</v>
       </c>
       <c r="E67" t="s">
         <v>27</v>
@@ -1606,13 +1609,13 @@
         <v>5</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="C68">
-        <v>1</v>
+        <v>0.96</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>1.01</v>
       </c>
       <c r="E68" t="s">
         <v>27</v>
@@ -1620,16 +1623,16 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B69">
-        <v>0.93</v>
+        <v>0.21</v>
       </c>
       <c r="C69">
-        <v>0.92</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D69">
-        <v>0.95</v>
+        <v>0.32</v>
       </c>
       <c r="E69" t="s">
         <v>27</v>
@@ -1640,13 +1643,13 @@
         <v>6</v>
       </c>
       <c r="B70">
-        <v>0.55000000000000004</v>
+        <v>0.59</v>
       </c>
       <c r="C70">
-        <v>0.43</v>
+        <v>0.45</v>
       </c>
       <c r="D70">
-        <v>0.7</v>
+        <v>0.77</v>
       </c>
       <c r="E70" t="s">
         <v>27</v>
@@ -1657,13 +1660,13 @@
         <v>31</v>
       </c>
       <c r="B71">
-        <v>0.87</v>
+        <v>0.17</v>
       </c>
       <c r="C71">
-        <v>0.84</v>
+        <v>0.12</v>
       </c>
       <c r="D71">
-        <v>0.89</v>
+        <v>0.23</v>
       </c>
       <c r="E71" t="s">
         <v>27</v>
@@ -2907,7 +2910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>